<commit_message>
Added Crowdfunding_df.ipynb and campaign.csv files
</commit_message>
<xml_diff>
--- a/crowdfunding.xlsx
+++ b/crowdfunding.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/25dd825479618544/Desktop/Data Bootcamp Class Folder/Github Repositories/Crowdfunding-ETL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{D7E51A4B-2461-4256-8A90-9F0FD044C427}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5A47DDE4-6D5D-4F87-840F-10AA44F5B1D4}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{D7E51A4B-2461-4256-8A90-9F0FD044C427}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{912779C6-F237-40B2-9E89-03CA0E871CF6}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="crowdfunding_info" sheetId="1" r:id="rId1"/>
@@ -9155,10 +9155,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -9175,6 +9178,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9500,8 +9507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -53574,8 +53581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A1004"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -53599,7 +53606,7 @@
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>2029</v>
       </c>
     </row>

</xml_diff>